<commit_message>
new moose transect transform
</commit_message>
<xml_diff>
--- a/utils/templates/observations/transform/output/dwcWorkbook_fixed_with_mark_2.xlsx
+++ b/utils/templates/observations/transform/output/dwcWorkbook_fixed_with_mark_2.xlsx
@@ -439,7 +439,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -451,9 +451,6 @@
       <c r="B1" t="str">
         <v>eventDate</v>
       </c>
-      <c r="C1" t="str">
-        <v>eventRemarks</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -462,13 +459,10 @@
       <c r="B2" t="str">
         <v>31/Jan/16</v>
       </c>
-      <c r="C2" t="str">
-        <v>have an observation</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -583,7 +577,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -664,19 +658,16 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B5" t="str">
-        <v>MU 749:Lowland:1:0:antler-configuration</v>
+        <v>MU 749:Lowland:1:0:sign-type</v>
       </c>
       <c r="C5" t="str">
-        <v>Antler Configuration</v>
+        <v>Sign Type</v>
       </c>
       <c r="D5" t="str">
         <v/>
       </c>
       <c r="E5" t="str">
-        <v>Spike/Fork</v>
-      </c>
-      <c r="F5" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
+        <v>Bed</v>
       </c>
     </row>
     <row r="6">
@@ -684,19 +675,16 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B6" t="str">
-        <v>MU 749:Lowland:1:0:sign-type</v>
+        <v>MU 749:Lowland:1:0:sign-count</v>
       </c>
       <c r="C6" t="str">
-        <v>Sign Type</v>
+        <v>Sign Count</v>
       </c>
       <c r="D6" t="str">
         <v/>
       </c>
       <c r="E6" t="str">
-        <v>Bed</v>
-      </c>
-      <c r="F6" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -704,19 +692,16 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B7" t="str">
-        <v>MU 749:Lowland:1:0:sign-count</v>
+        <v>MU 749:Lowland:1:0:age-of-sign</v>
       </c>
       <c r="C7" t="str">
-        <v>Sign Count</v>
+        <v>Age of Sign</v>
       </c>
       <c r="D7" t="str">
         <v/>
       </c>
       <c r="E7" t="str">
-        <v>1</v>
-      </c>
-      <c r="F7" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
+        <v>Old</v>
       </c>
     </row>
     <row r="8">
@@ -724,19 +709,16 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B8" t="str">
-        <v>MU 749:Lowland:1:0:age-of-sign</v>
+        <v>MU 749:Lowland:1:0:veg-cover</v>
       </c>
       <c r="C8" t="str">
-        <v>Age of Sign</v>
+        <v>Veg Cover</v>
       </c>
       <c r="D8" t="str">
-        <v/>
+        <v>%</v>
       </c>
       <c r="E8" t="str">
-        <v>Old</v>
-      </c>
-      <c r="F8" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -744,19 +726,16 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B9" t="str">
-        <v>MU 749:Lowland:1:0:veg-cover</v>
+        <v>MU 749:Lowland:1:0:snow-cover</v>
       </c>
       <c r="C9" t="str">
-        <v>Veg Cover</v>
+        <v>Snow Cover</v>
       </c>
       <c r="D9" t="str">
         <v>%</v>
       </c>
       <c r="E9" t="str">
-        <v>2</v>
-      </c>
-      <c r="F9" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -764,19 +743,16 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B10" t="str">
-        <v>MU 749:Lowland:1:0:snow-cover</v>
+        <v>MU 749:Lowland:1:0:activity</v>
       </c>
       <c r="C10" t="str">
-        <v>Snow Cover</v>
+        <v>Activity</v>
       </c>
       <c r="D10" t="str">
-        <v>%</v>
+        <v/>
       </c>
       <c r="E10" t="str">
-        <v>3</v>
-      </c>
-      <c r="F10" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
+        <v>Bedding</v>
       </c>
     </row>
     <row r="11">
@@ -784,19 +760,16 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B11" t="str">
-        <v>MU 749:Lowland:1:0:activity</v>
+        <v>MU 749:Lowland:1:0:number-of-marked-animals-observed</v>
       </c>
       <c r="C11" t="str">
-        <v>Activity</v>
+        <v>Number of Marked Animals Observed</v>
       </c>
       <c r="D11" t="str">
         <v/>
       </c>
       <c r="E11" t="str">
-        <v>Bedding</v>
-      </c>
-      <c r="F11" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -804,19 +777,16 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B12" t="str">
-        <v>MU 749:Lowland:1:0:number-of-marked-animals-observed</v>
+        <v>MU 749:Lowland:1:0:survey-or-telemetry-search</v>
       </c>
       <c r="C12" t="str">
-        <v>Number of Marked Animals Observed</v>
+        <v>Survey or Telemetry Search</v>
       </c>
       <c r="D12" t="str">
         <v/>
       </c>
       <c r="E12" t="str">
-        <v>4</v>
-      </c>
-      <c r="F12" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
+        <v>Survey</v>
       </c>
     </row>
     <row r="13">
@@ -824,19 +794,16 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B13" t="str">
-        <v>MU 749:Lowland:1:0:survey-or-telemetry-search</v>
+        <v>MU 749:Lowland:1:0:photos</v>
       </c>
       <c r="C13" t="str">
-        <v>Survey or Telemetry Search</v>
+        <v>Photos</v>
       </c>
       <c r="D13" t="str">
         <v/>
       </c>
       <c r="E13" t="str">
-        <v>Survey</v>
-      </c>
-      <c r="F13" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
+        <v>some photo id</v>
       </c>
     </row>
     <row r="14">
@@ -844,44 +811,24 @@
         <v>MU 749:Lowland:1:0</v>
       </c>
       <c r="B14" t="str">
-        <v>MU 749:Lowland:1:0:photos</v>
+        <v>MU 749:Lowland:1:0:antler-configuration</v>
       </c>
       <c r="C14" t="str">
-        <v>Photos</v>
+        <v>Antler Configuration</v>
       </c>
       <c r="D14" t="str">
         <v/>
       </c>
       <c r="E14" t="str">
-        <v>some photo id</v>
+        <v>Spike/Fork</v>
       </c>
       <c r="F14" t="str">
         <v>MU 749:Lowland:1:0:0</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>MU 749:Lowland:1:0</v>
-      </c>
-      <c r="B15" t="str">
-        <v>MU 749:Lowland:1:0:observation-comments</v>
-      </c>
-      <c r="C15" t="str">
-        <v>Observation Comments</v>
-      </c>
-      <c r="D15" t="str">
-        <v/>
-      </c>
-      <c r="E15" t="str">
-        <v>have an observation</v>
-      </c>
-      <c r="F15" t="str">
-        <v>MU 749:Lowland:1:0:0</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F14"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>